<commit_message>
changing percent change depending on users input
</commit_message>
<xml_diff>
--- a/modified_sheets/marks1.xlsx
+++ b/modified_sheets/marks1.xlsx
@@ -658,7 +658,7 @@
         <v>70</v>
       </c>
       <c r="F2" t="n">
-        <v>31.5</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="3">
@@ -680,7 +680,7 @@
         <v>69</v>
       </c>
       <c r="F3" t="n">
-        <v>60.2</v>
+        <v>46.44</v>
       </c>
     </row>
     <row r="4">
@@ -702,7 +702,7 @@
         <v>98</v>
       </c>
       <c r="F4" t="n">
-        <v>33.59999999999999</v>
+        <v>25.92</v>
       </c>
     </row>
     <row r="5">
@@ -724,7 +724,7 @@
         <v>79</v>
       </c>
       <c r="F5" t="n">
-        <v>39.9</v>
+        <v>30.78</v>
       </c>
     </row>
     <row r="6">
@@ -746,7 +746,7 @@
         <v>86</v>
       </c>
       <c r="F6" t="n">
-        <v>59.49999999999999</v>
+        <v>45.90000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -768,7 +768,7 @@
         <v>71</v>
       </c>
       <c r="F7" t="n">
-        <v>52.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="8">
@@ -790,7 +790,7 @@
         <v>92</v>
       </c>
       <c r="F8" t="n">
-        <v>40.59999999999999</v>
+        <v>31.32</v>
       </c>
     </row>
     <row r="9">
@@ -812,7 +812,7 @@
         <v>55</v>
       </c>
       <c r="F9" t="n">
-        <v>24.5</v>
+        <v>18.9</v>
       </c>
     </row>
     <row r="10">
@@ -834,7 +834,7 @@
         <v>94</v>
       </c>
       <c r="F10" t="n">
-        <v>28</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="11">
@@ -856,7 +856,7 @@
         <v>57</v>
       </c>
       <c r="F11" t="n">
-        <v>64.39999999999999</v>
+        <v>49.68000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -878,7 +878,7 @@
         <v>98</v>
       </c>
       <c r="F12" t="n">
-        <v>66.5</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="13">
@@ -900,7 +900,7 @@
         <v>34</v>
       </c>
       <c r="F13" t="n">
-        <v>62.3</v>
+        <v>48.06</v>
       </c>
     </row>
     <row r="14">
@@ -922,7 +922,7 @@
         <v>96</v>
       </c>
       <c r="F14" t="n">
-        <v>36.4</v>
+        <v>28.08</v>
       </c>
     </row>
     <row r="15">
@@ -944,7 +944,7 @@
         <v>76</v>
       </c>
       <c r="F15" t="n">
-        <v>40.59999999999999</v>
+        <v>31.32</v>
       </c>
     </row>
     <row r="16">
@@ -966,7 +966,7 @@
         <v>45</v>
       </c>
       <c r="F16" t="n">
-        <v>43.4</v>
+        <v>33.48</v>
       </c>
     </row>
     <row r="17">
@@ -988,7 +988,7 @@
         <v>60</v>
       </c>
       <c r="F17" t="n">
-        <v>69.3</v>
+        <v>53.46</v>
       </c>
     </row>
     <row r="18">
@@ -1010,7 +1010,7 @@
         <v>71</v>
       </c>
       <c r="F18" t="n">
-        <v>30.1</v>
+        <v>23.22</v>
       </c>
     </row>
     <row r="19">
@@ -1032,7 +1032,7 @@
         <v>36</v>
       </c>
       <c r="F19" t="n">
-        <v>49.7</v>
+        <v>38.34</v>
       </c>
     </row>
     <row r="20">
@@ -1054,7 +1054,7 @@
         <v>78</v>
       </c>
       <c r="F20" t="n">
-        <v>58.8</v>
+        <v>45.36</v>
       </c>
     </row>
     <row r="21">
@@ -1076,7 +1076,7 @@
         <v>98</v>
       </c>
       <c r="F21" t="n">
-        <v>44.09999999999999</v>
+        <v>34.02</v>
       </c>
     </row>
     <row r="22">
@@ -1098,7 +1098,7 @@
         <v>50</v>
       </c>
       <c r="F22" t="n">
-        <v>47.59999999999999</v>
+        <v>36.72</v>
       </c>
     </row>
     <row r="23">
@@ -1120,7 +1120,7 @@
         <v>95</v>
       </c>
       <c r="F23" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
@@ -1142,7 +1142,7 @@
         <v>96</v>
       </c>
       <c r="F24" t="n">
-        <v>31.5</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="25">
@@ -1164,7 +1164,7 @@
         <v>67</v>
       </c>
       <c r="F25" t="n">
-        <v>37.8</v>
+        <v>29.16</v>
       </c>
     </row>
     <row r="26">
@@ -1186,7 +1186,7 @@
         <v>45</v>
       </c>
       <c r="F26" t="n">
-        <v>39.2</v>
+        <v>30.24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>